<commit_message>
Updated Purchase Order, Purchase Invoice and Purchase Voucher
</commit_message>
<xml_diff>
--- a/assets/images/propertygaga/purchase-invoice-open.xlsx
+++ b/assets/images/propertygaga/purchase-invoice-open.xlsx
@@ -12,7 +12,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
+  <si>
+    <t>Perbadanan Pengurusan Relau Vista Apartment</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color indexed="9"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Block 2-G-01, Lebuh Relau 6, 11900 Bayan Lepas, Penang, Malaysia +Tel/Fax : 04-6425118 Email: </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="13"/>
+        <color indexed="13"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>mcrelauvista@gmail.com</t>
+    </r>
+  </si>
   <si>
     <t>Open Purchase Invoices (Ready for payment)</t>
   </si>
@@ -36,10 +59,10 @@
     <t>Task ID</t>
   </si>
   <si>
-    <t>P.O.</t>
-  </si>
-  <si>
-    <t>Vendor</t>
+    <t>P.O. No.</t>
+  </si>
+  <si>
+    <t>Payee / Vendor</t>
   </si>
   <si>
     <t>Reg. No.</t>
@@ -60,13 +83,16 @@
     <t>Amount (RM)</t>
   </si>
   <si>
-    <t xml:space="preserve">Payment (RM)	</t>
+    <t>Payment (RM)</t>
   </si>
   <si>
     <t>For Asset</t>
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>20/2/2025, 01:32:34</t>
   </si>
   <si>
     <t>OT022</t>
@@ -97,8 +123,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="59" formatCode="d/m/yy"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -134,6 +161,12 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <u val="single"/>
+      <sz val="13"/>
+      <color indexed="13"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <b val="1"/>
       <sz val="12"/>
       <color indexed="12"/>
@@ -141,18 +174,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="14"/>
+      <color indexed="15"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color indexed="14"/>
-      <name val="Avenir Next"/>
-    </font>
-    <font>
       <b val="1"/>
-      <sz val="11"/>
-      <color indexed="14"/>
+      <sz val="15"/>
+      <color indexed="15"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -171,18 +199,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="13"/>
+        <fgColor indexed="14"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="17"/>
+        <fgColor indexed="18"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -197,13 +225,6 @@
       <bottom>
         <color indexed="9"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -267,12 +288,33 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right>
+        <color indexed="9"/>
+      </right>
+      <top>
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left>
         <color indexed="9"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
+      <right>
+        <color indexed="9"/>
+      </right>
+      <top>
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -309,8 +351,8 @@
       <left style="thin">
         <color indexed="12"/>
       </left>
-      <right>
-        <color indexed="9"/>
+      <right style="thin">
+        <color indexed="11"/>
       </right>
       <top>
         <color indexed="9"/>
@@ -321,9 +363,54 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
-        <color indexed="15"/>
+        <color indexed="16"/>
       </right>
       <top style="medium">
         <color indexed="12"/>
@@ -333,10 +420,10 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="15"/>
+        <color indexed="16"/>
       </left>
       <right style="thin">
-        <color indexed="15"/>
+        <color indexed="16"/>
       </right>
       <top style="medium">
         <color indexed="12"/>
@@ -346,30 +433,34 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="15"/>
+        <color indexed="16"/>
       </left>
       <right style="thin">
-        <color indexed="15"/>
+        <color indexed="16"/>
       </right>
-      <top>
-        <color indexed="9"/>
+      <top style="medium">
+        <color indexed="11"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="15"/>
+        <color indexed="16"/>
       </left>
-      <right/>
-      <top/>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="15"/>
+        <color indexed="16"/>
       </right>
       <top/>
       <bottom/>
@@ -377,10 +468,10 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="15"/>
+        <color indexed="16"/>
       </left>
       <right style="thin">
-        <color indexed="15"/>
+        <color indexed="16"/>
       </right>
       <top/>
       <bottom/>
@@ -389,7 +480,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="15"/>
+        <color indexed="16"/>
       </right>
       <top/>
       <bottom style="medium">
@@ -399,10 +490,10 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="15"/>
+        <color indexed="16"/>
       </left>
       <right style="thin">
-        <color indexed="15"/>
+        <color indexed="16"/>
       </right>
       <top/>
       <bottom style="medium">
@@ -416,7 +507,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -429,11 +520,11 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
@@ -441,91 +532,115 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="5" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="8" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -555,6 +670,7 @@
       <rgbColor rgb="ff444344"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="fffefefe"/>
+      <rgbColor rgb="ff0000ff"/>
       <rgbColor rgb="ff415baa"/>
       <rgbColor rgb="ff090547"/>
       <rgbColor rgb="ffebe8e3"/>
@@ -1624,7 +1740,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q20"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1632,7 +1748,7 @@
   <cols>
     <col min="1" max="1" width="14.1719" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.1719" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1719" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.3203" style="1" customWidth="1"/>
     <col min="4" max="4" width="14.1719" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.1719" style="1" customWidth="1"/>
     <col min="6" max="6" width="14.1719" style="1" customWidth="1"/>
@@ -1644,10 +1760,9 @@
     <col min="12" max="12" width="13.8516" style="1" customWidth="1"/>
     <col min="13" max="13" width="13.8516" style="1" customWidth="1"/>
     <col min="14" max="14" width="16.6875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="25.7812" style="1" customWidth="1"/>
-    <col min="16" max="16" width="13.8516" style="1" customWidth="1"/>
-    <col min="17" max="17" width="21.6719" style="1" customWidth="1"/>
-    <col min="18" max="256" width="21.6719" style="1" customWidth="1"/>
+    <col min="15" max="15" width="20.6641" style="1" customWidth="1"/>
+    <col min="16" max="16" width="27.9688" style="1" customWidth="1"/>
+    <col min="17" max="256" width="21.6719" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="9" customHeight="1">
@@ -1667,446 +1782,513 @@
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
-      <c r="Q1" s="4"/>
-    </row>
-    <row r="2" ht="21" customHeight="1">
-      <c r="A2" t="s" s="5">
+    </row>
+    <row r="2" ht="20" customHeight="1">
+      <c r="A2" t="s" s="4">
         <v>0</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="9"/>
-    </row>
-    <row r="3" ht="17" customHeight="1">
-      <c r="A3" t="s" s="10">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+    </row>
+    <row r="3" ht="31.1" customHeight="1">
+      <c r="A3" t="s" s="8">
         <v>1</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="9"/>
-    </row>
-    <row r="4" ht="36.85" customHeight="1">
-      <c r="A4" t="s" s="11">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+    </row>
+    <row r="4" ht="20" customHeight="1">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+    </row>
+    <row r="5" ht="20" customHeight="1">
+      <c r="A5" t="s" s="4">
         <v>2</v>
       </c>
-      <c r="B4" t="s" s="12">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+    </row>
+    <row r="6" ht="15.1" customHeight="1">
+      <c r="A6" t="s" s="8">
         <v>3</v>
       </c>
-      <c r="C4" t="s" s="12">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+    </row>
+    <row r="7" ht="15.6" customHeight="1">
+      <c r="A7" s="8"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+    </row>
+    <row r="8" ht="36.85" customHeight="1">
+      <c r="A8" t="s" s="11">
         <v>4</v>
       </c>
-      <c r="D4" t="s" s="12">
+      <c r="B8" t="s" s="12">
         <v>5</v>
       </c>
-      <c r="E4" t="s" s="12">
+      <c r="C8" t="s" s="12">
         <v>6</v>
       </c>
-      <c r="F4" t="s" s="12">
+      <c r="D8" t="s" s="12">
         <v>7</v>
       </c>
-      <c r="G4" t="s" s="13">
+      <c r="E8" t="s" s="12">
         <v>8</v>
       </c>
-      <c r="H4" t="s" s="14">
+      <c r="F8" t="s" s="13">
         <v>9</v>
       </c>
-      <c r="I4" t="s" s="14">
+      <c r="G8" t="s" s="14">
         <v>10</v>
       </c>
-      <c r="J4" t="s" s="14">
+      <c r="H8" t="s" s="15">
         <v>11</v>
       </c>
-      <c r="K4" t="s" s="14">
+      <c r="I8" t="s" s="15">
         <v>12</v>
       </c>
-      <c r="L4" t="s" s="14">
+      <c r="J8" t="s" s="15">
         <v>13</v>
       </c>
-      <c r="M4" t="s" s="14">
+      <c r="K8" t="s" s="15">
         <v>14</v>
       </c>
-      <c r="N4" t="s" s="14">
+      <c r="L8" t="s" s="15">
         <v>15</v>
       </c>
-      <c r="O4" t="s" s="14">
+      <c r="M8" t="s" s="16">
         <v>16</v>
       </c>
-      <c r="P4" t="s" s="14">
+      <c r="N8" t="s" s="17">
         <v>17</v>
       </c>
-      <c r="Q4" s="9"/>
-    </row>
-    <row r="5" ht="23" customHeight="1">
-      <c r="A5" s="15">
+      <c r="O8" t="s" s="15">
+        <v>18</v>
+      </c>
+      <c r="P8" t="s" s="15">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" ht="23" customHeight="1">
+      <c r="A9" s="18">
         <v>3535</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B9" s="19">
         <v>6436436</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" t="s" s="18">
-        <v>18</v>
-      </c>
-      <c r="F5" t="s" s="18">
-        <v>19</v>
-      </c>
-      <c r="G5" t="s" s="18">
+      <c r="C9" t="s" s="20">
         <v>20</v>
       </c>
-      <c r="H5" t="s" s="19">
+      <c r="D9" s="21">
+        <v>44246</v>
+      </c>
+      <c r="E9" t="s" s="20">
         <v>21</v>
       </c>
-      <c r="I5" t="s" s="19">
+      <c r="F9" t="s" s="20">
         <v>22</v>
       </c>
-      <c r="J5" t="s" s="19">
+      <c r="G9" t="s" s="22">
         <v>23</v>
       </c>
-      <c r="K5" t="s" s="19">
+      <c r="H9" t="s" s="23">
         <v>24</v>
       </c>
-      <c r="L5" s="20">
+      <c r="I9" t="s" s="23">
+        <v>25</v>
+      </c>
+      <c r="J9" t="s" s="23">
+        <v>26</v>
+      </c>
+      <c r="K9" t="s" s="23">
+        <v>27</v>
+      </c>
+      <c r="L9" s="24">
         <v>1</v>
       </c>
-      <c r="M5" s="20">
+      <c r="M9" s="25">
         <v>500</v>
       </c>
-      <c r="N5" s="20">
+      <c r="N9" s="26">
         <v>500</v>
       </c>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="22"/>
-    </row>
-    <row r="6" ht="22" customHeight="1">
-      <c r="A6" s="23"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="25"/>
-      <c r="O6" s="25"/>
-      <c r="P6" s="25"/>
-      <c r="Q6" s="22"/>
-    </row>
-    <row r="7" ht="22" customHeight="1">
-      <c r="A7" s="26"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="28"/>
-      <c r="P7" s="28"/>
-      <c r="Q7" s="22"/>
-    </row>
-    <row r="8" ht="22" customHeight="1">
-      <c r="A8" s="23"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="25"/>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="22"/>
-    </row>
-    <row r="9" ht="22" customHeight="1">
-      <c r="A9" s="26"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="28"/>
-      <c r="P9" s="28"/>
-      <c r="Q9" s="22"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="27"/>
     </row>
     <row r="10" ht="22" customHeight="1">
-      <c r="A10" s="23"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="25"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="22"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="30"/>
     </row>
     <row r="11" ht="22" customHeight="1">
-      <c r="A11" s="26"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="28"/>
-      <c r="N11" s="28"/>
-      <c r="O11" s="28"/>
-      <c r="P11" s="28"/>
-      <c r="Q11" s="22"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="35"/>
+      <c r="N11" s="35"/>
+      <c r="O11" s="34"/>
+      <c r="P11" s="34"/>
     </row>
     <row r="12" ht="22" customHeight="1">
-      <c r="A12" s="23"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="22"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="30"/>
     </row>
     <row r="13" ht="22" customHeight="1">
-      <c r="A13" s="26"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="28"/>
-      <c r="N13" s="28"/>
-      <c r="O13" s="28"/>
-      <c r="P13" s="28"/>
-      <c r="Q13" s="22"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="35"/>
+      <c r="N13" s="35"/>
+      <c r="O13" s="34"/>
+      <c r="P13" s="34"/>
     </row>
     <row r="14" ht="22" customHeight="1">
-      <c r="A14" s="23"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="24"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="25"/>
-      <c r="P14" s="25"/>
-      <c r="Q14" s="22"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="31"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="30"/>
     </row>
     <row r="15" ht="22" customHeight="1">
-      <c r="A15" s="26"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="27"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
-      <c r="O15" s="28"/>
-      <c r="P15" s="28"/>
-      <c r="Q15" s="22"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="34"/>
+      <c r="M15" s="35"/>
+      <c r="N15" s="35"/>
+      <c r="O15" s="34"/>
+      <c r="P15" s="34"/>
     </row>
     <row r="16" ht="22" customHeight="1">
-      <c r="A16" s="23"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="24"/>
-      <c r="L16" s="25"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="25"/>
-      <c r="O16" s="25"/>
-      <c r="P16" s="25"/>
-      <c r="Q16" s="22"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="31"/>
+      <c r="N16" s="31"/>
+      <c r="O16" s="30"/>
+      <c r="P16" s="30"/>
     </row>
     <row r="17" ht="22" customHeight="1">
-      <c r="A17" s="26"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="28"/>
-      <c r="N17" s="28"/>
-      <c r="O17" s="28"/>
-      <c r="P17" s="28"/>
-      <c r="Q17" s="22"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="34"/>
+      <c r="M17" s="35"/>
+      <c r="N17" s="35"/>
+      <c r="O17" s="34"/>
+      <c r="P17" s="34"/>
     </row>
     <row r="18" ht="22" customHeight="1">
-      <c r="A18" s="23"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="24"/>
-      <c r="L18" s="25"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="25"/>
-      <c r="O18" s="25"/>
-      <c r="P18" s="25"/>
-      <c r="Q18" s="22"/>
-    </row>
-    <row r="19" ht="23" customHeight="1">
-      <c r="A19" s="29"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
-      <c r="K19" s="30"/>
-      <c r="L19" s="31"/>
-      <c r="M19" s="31"/>
-      <c r="N19" s="31"/>
-      <c r="O19" s="31"/>
-      <c r="P19" s="31"/>
-      <c r="Q19" s="22"/>
-    </row>
-    <row r="20" ht="23" customHeight="1">
-      <c r="A20" s="32"/>
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33"/>
-      <c r="K20" s="33"/>
-      <c r="L20" t="s" s="34">
-        <v>25</v>
-      </c>
-      <c r="M20" s="35">
+      <c r="A18" s="28"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="31"/>
+      <c r="O18" s="30"/>
+      <c r="P18" s="30"/>
+    </row>
+    <row r="19" ht="22" customHeight="1">
+      <c r="A19" s="32"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="33"/>
+      <c r="L19" s="34"/>
+      <c r="M19" s="35"/>
+      <c r="N19" s="35"/>
+      <c r="O19" s="34"/>
+      <c r="P19" s="34"/>
+    </row>
+    <row r="20" ht="22" customHeight="1">
+      <c r="A20" s="28"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="31"/>
+      <c r="N20" s="31"/>
+      <c r="O20" s="30"/>
+      <c r="P20" s="30"/>
+    </row>
+    <row r="21" ht="22" customHeight="1">
+      <c r="A21" s="32"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="35"/>
+      <c r="N21" s="35"/>
+      <c r="O21" s="34"/>
+      <c r="P21" s="34"/>
+    </row>
+    <row r="22" ht="22" customHeight="1">
+      <c r="A22" s="28"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="30"/>
+      <c r="M22" s="31"/>
+      <c r="N22" s="31"/>
+      <c r="O22" s="30"/>
+      <c r="P22" s="30"/>
+    </row>
+    <row r="23" ht="23" customHeight="1">
+      <c r="A23" s="36"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="37"/>
+      <c r="L23" s="38"/>
+      <c r="M23" s="39"/>
+      <c r="N23" s="39"/>
+      <c r="O23" s="38"/>
+      <c r="P23" s="38"/>
+    </row>
+    <row r="24" ht="23" customHeight="1">
+      <c r="A24" s="40"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="41"/>
+      <c r="J24" s="41"/>
+      <c r="K24" s="41"/>
+      <c r="L24" t="s" s="42">
+        <v>28</v>
+      </c>
+      <c r="M24" s="43">
         <v>10000</v>
       </c>
-      <c r="N20" s="35">
+      <c r="N24" s="43">
         <v>10000</v>
       </c>
-      <c r="O20" s="36"/>
-      <c r="P20" s="36"/>
-      <c r="Q20" s="22"/>
+      <c r="O24" s="44"/>
+      <c r="P24" s="44"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="7">
+    <mergeCell ref="A7:P7"/>
     <mergeCell ref="A3:P3"/>
     <mergeCell ref="A2:P2"/>
+    <mergeCell ref="A4:P4"/>
+    <mergeCell ref="A5:P5"/>
+    <mergeCell ref="A6:P6"/>
     <mergeCell ref="A1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A5:P20">
+  <conditionalFormatting sqref="A9:P24">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal" stopIfTrue="1">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" location="" tooltip="" display=""/>
+  </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.8" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>
   <headerFooter>

</xml_diff>

<commit_message>
Updated Purchase Invoice pages
</commit_message>
<xml_diff>
--- a/assets/images/propertygaga/purchase-invoice-open.xlsx
+++ b/assets/images/propertygaga/purchase-invoice-open.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
   <si>
     <t>Perbadanan Pengurusan Relau Vista Apartment</t>
   </si>
@@ -23,14 +23,22 @@
         <color indexed="9"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t xml:space="preserve">Block 2-G-01, Lebuh Relau 6, 11900 Bayan Lepas, Penang, Malaysia -Tel/Fax : 04-6425118 Email: </t>
+      <t xml:space="preserve">Block 2-G-01, Lebuh Relau 6, 11900 Bayan Lepas, Penang, Malaysia
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color indexed="9"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Tel/Fax : 04-6425118 Email: </t>
     </r>
     <r>
       <rPr>
         <u val="single"/>
         <sz val="13"/>
-        <color indexed="13"/>
+        <color indexed="14"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>mcrelauvista@gmail.com</t>
@@ -83,7 +91,7 @@
     <t>Amount (RM)</t>
   </si>
   <si>
-    <t>Payment (RM)</t>
+    <t>Amount Paid (RM)</t>
   </si>
   <si>
     <t>For Asset</t>
@@ -92,6 +100,9 @@
     <t>Notes</t>
   </si>
   <si>
+    <t>Ready to pay</t>
+  </si>
+  <si>
     <t>20/2/2025, 01:32:34</t>
   </si>
   <si>
@@ -114,6 +125,12 @@
   </si>
   <si>
     <t>Air Cons</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>YES</t>
   </si>
   <si>
     <t>Total</t>
@@ -163,28 +180,28 @@
     <font>
       <u val="single"/>
       <sz val="13"/>
-      <color indexed="13"/>
+      <color indexed="14"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b val="1"/>
       <sz val="12"/>
-      <color indexed="12"/>
+      <color indexed="13"/>
       <name val="Arial"/>
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="15"/>
+      <color indexed="16"/>
       <name val="Arial"/>
     </font>
     <font>
       <b val="1"/>
       <sz val="15"/>
-      <color indexed="15"/>
+      <color indexed="16"/>
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -199,18 +216,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="14"/>
+        <fgColor indexed="15"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="18"/>
+        <fgColor indexed="19"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="20"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -219,27 +242,34 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom>
-        <color indexed="9"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left>
-        <color indexed="9"/>
-      </left>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="12"/>
       </right>
-      <top>
-        <color indexed="9"/>
+      <top style="thin">
+        <color indexed="12"/>
       </top>
-      <bottom>
-        <color indexed="9"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -247,88 +277,76 @@
         <color indexed="12"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
-      <top>
-        <color indexed="9"/>
-      </top>
-      <bottom>
-        <color indexed="9"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
-      <right>
-        <color indexed="9"/>
+      <right style="thin">
+        <color indexed="13"/>
       </right>
-      <top>
-        <color indexed="9"/>
-      </top>
-      <bottom>
-        <color indexed="9"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left>
-        <color indexed="9"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
       </left>
-      <right>
-        <color indexed="9"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
       </right>
-      <top>
-        <color indexed="9"/>
-      </top>
-      <bottom>
-        <color indexed="9"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
-      <right>
-        <color indexed="9"/>
-      </right>
-      <top>
-        <color indexed="9"/>
-      </top>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left>
-        <color indexed="9"/>
-      </left>
-      <right>
-        <color indexed="9"/>
-      </right>
-      <top>
-        <color indexed="9"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left>
-        <color indexed="9"/>
-      </left>
+      <left/>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
-      <top>
-        <color indexed="9"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="12"/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -337,28 +355,37 @@
         <color indexed="12"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
-      <top>
-        <color indexed="9"/>
-      </top>
+      <top/>
       <bottom style="medium">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
       </right>
-      <top>
-        <color indexed="9"/>
-      </top>
+      <top/>
       <bottom style="medium">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -403,40 +430,102 @@
         <color indexed="11"/>
       </top>
       <bottom style="medium">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+      </left>
       <right style="thin">
-        <color indexed="16"/>
+        <color indexed="17"/>
       </right>
       <top style="medium">
+        <color indexed="13"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="17"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top style="medium">
+        <color indexed="13"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="17"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top style="medium">
+        <color indexed="11"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="17"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="12"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top style="medium">
+        <color indexed="13"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="16"/>
+        <color indexed="17"/>
       </left>
       <right style="thin">
-        <color indexed="16"/>
+        <color indexed="17"/>
       </right>
       <top style="medium">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="16"/>
+        <color indexed="17"/>
       </left>
       <right style="thin">
-        <color indexed="16"/>
+        <color indexed="17"/>
       </right>
       <top style="medium">
         <color indexed="11"/>
@@ -446,10 +535,10 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="16"/>
+        <color indexed="17"/>
       </left>
       <right style="thin">
-        <color indexed="16"/>
+        <color indexed="17"/>
       </right>
       <top style="thin">
         <color indexed="11"/>
@@ -458,9 +547,11 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
       <right style="thin">
-        <color indexed="16"/>
+        <color indexed="17"/>
       </right>
       <top/>
       <bottom/>
@@ -468,35 +559,67 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="16"/>
+        <color indexed="17"/>
       </left>
       <right style="thin">
-        <color indexed="16"/>
+        <color indexed="17"/>
       </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
       <right style="thin">
-        <color indexed="16"/>
+        <color indexed="17"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="16"/>
+        <color indexed="17"/>
       </left>
       <right style="thin">
-        <color indexed="16"/>
+        <color indexed="17"/>
       </right>
       <top/>
       <bottom style="medium">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top style="medium">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="17"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top style="medium">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
         <color indexed="12"/>
       </bottom>
       <diagonal/>
@@ -507,147 +630,194 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="3" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="3" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="59" fontId="8" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="8" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="8" fillId="4" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="5" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="ffd23600"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="ffd23600"/>
@@ -669,12 +839,14 @@
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ff444344"/>
       <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="fffefefe"/>
       <rgbColor rgb="ff0000ff"/>
       <rgbColor rgb="ff415baa"/>
       <rgbColor rgb="ff090547"/>
       <rgbColor rgb="ffebe8e3"/>
       <rgbColor rgb="ffd23600"/>
+      <rgbColor rgb="ffeaeaea"/>
       <rgbColor rgb="ffeeeeee"/>
     </indexedColors>
   </colors>
@@ -912,10 +1084,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Superclarendon Light"/>
-            <a:ea typeface="Superclarendon Light"/>
-            <a:cs typeface="Superclarendon Light"/>
-            <a:sym typeface="Superclarendon Light"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1483,10 +1655,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Superclarendon Light"/>
-            <a:ea typeface="Superclarendon Light"/>
-            <a:cs typeface="Superclarendon Light"/>
-            <a:sym typeface="Superclarendon Light"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1740,7 +1912,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P24"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1748,21 +1920,22 @@
   <cols>
     <col min="1" max="1" width="14.1719" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.1719" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.3203" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.3516" style="1" customWidth="1"/>
     <col min="4" max="4" width="14.1719" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.1719" style="1" customWidth="1"/>
     <col min="6" max="6" width="14.1719" style="1" customWidth="1"/>
-    <col min="7" max="7" width="33.2578" style="1" customWidth="1"/>
+    <col min="7" max="7" width="33.3516" style="1" customWidth="1"/>
     <col min="8" max="8" width="13.8516" style="1" customWidth="1"/>
     <col min="9" max="9" width="13.8516" style="1" customWidth="1"/>
-    <col min="10" max="10" width="23.625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="23.6719" style="1" customWidth="1"/>
     <col min="11" max="11" width="13.8516" style="1" customWidth="1"/>
     <col min="12" max="12" width="13.8516" style="1" customWidth="1"/>
     <col min="13" max="13" width="13.8516" style="1" customWidth="1"/>
-    <col min="14" max="14" width="16.6875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="20.6641" style="1" customWidth="1"/>
-    <col min="16" max="16" width="27.9688" style="1" customWidth="1"/>
-    <col min="17" max="256" width="21.6719" style="1" customWidth="1"/>
+    <col min="14" max="14" width="18.6953" style="1" customWidth="1"/>
+    <col min="15" max="15" width="20.6719" style="1" customWidth="1"/>
+    <col min="16" max="16" width="28" style="1" customWidth="1"/>
+    <col min="17" max="17" width="17.3281" style="1" customWidth="1"/>
+    <col min="18" max="256" width="21.6719" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="9" customHeight="1">
@@ -1773,516 +1946,579 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="4"/>
     </row>
     <row r="2" ht="20" customHeight="1">
-      <c r="A2" t="s" s="4">
+      <c r="A2" t="s" s="5">
         <v>0</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="9"/>
     </row>
     <row r="3" ht="31.1" customHeight="1">
-      <c r="A3" t="s" s="8">
+      <c r="A3" t="s" s="10">
         <v>1</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="11"/>
     </row>
     <row r="4" ht="20" customHeight="1">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="9"/>
     </row>
     <row r="5" ht="20" customHeight="1">
-      <c r="A5" t="s" s="4">
+      <c r="A5" t="s" s="5">
         <v>2</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="9"/>
     </row>
     <row r="6" ht="15.1" customHeight="1">
-      <c r="A6" t="s" s="8">
+      <c r="A6" t="s" s="10">
         <v>3</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="11"/>
     </row>
     <row r="7" ht="15.6" customHeight="1">
-      <c r="A7" s="8"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="14"/>
     </row>
     <row r="8" ht="36.85" customHeight="1">
-      <c r="A8" t="s" s="11">
+      <c r="A8" t="s" s="15">
         <v>4</v>
       </c>
-      <c r="B8" t="s" s="12">
+      <c r="B8" t="s" s="16">
         <v>5</v>
       </c>
-      <c r="C8" t="s" s="12">
+      <c r="C8" t="s" s="16">
         <v>6</v>
       </c>
-      <c r="D8" t="s" s="12">
+      <c r="D8" t="s" s="16">
         <v>7</v>
       </c>
-      <c r="E8" t="s" s="12">
+      <c r="E8" t="s" s="16">
         <v>8</v>
       </c>
-      <c r="F8" t="s" s="13">
+      <c r="F8" t="s" s="17">
         <v>9</v>
       </c>
-      <c r="G8" t="s" s="14">
+      <c r="G8" t="s" s="18">
         <v>10</v>
       </c>
-      <c r="H8" t="s" s="15">
+      <c r="H8" t="s" s="19">
         <v>11</v>
       </c>
-      <c r="I8" t="s" s="15">
+      <c r="I8" t="s" s="19">
         <v>12</v>
       </c>
-      <c r="J8" t="s" s="15">
+      <c r="J8" t="s" s="19">
         <v>13</v>
       </c>
-      <c r="K8" t="s" s="15">
+      <c r="K8" t="s" s="19">
         <v>14</v>
       </c>
-      <c r="L8" t="s" s="15">
+      <c r="L8" t="s" s="19">
         <v>15</v>
       </c>
-      <c r="M8" t="s" s="16">
+      <c r="M8" t="s" s="20">
         <v>16</v>
       </c>
-      <c r="N8" t="s" s="17">
+      <c r="N8" t="s" s="21">
         <v>17</v>
       </c>
-      <c r="O8" t="s" s="15">
+      <c r="O8" t="s" s="19">
         <v>18</v>
       </c>
-      <c r="P8" t="s" s="15">
+      <c r="P8" t="s" s="19">
         <v>19</v>
+      </c>
+      <c r="Q8" t="s" s="19">
+        <v>20</v>
       </c>
     </row>
     <row r="9" ht="23" customHeight="1">
-      <c r="A9" s="18">
+      <c r="A9" s="22">
         <v>3535</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="23">
         <v>6436436</v>
       </c>
-      <c r="C9" t="s" s="20">
-        <v>20</v>
-      </c>
-      <c r="D9" s="21">
+      <c r="C9" t="s" s="24">
+        <v>21</v>
+      </c>
+      <c r="D9" s="25">
         <v>44246</v>
       </c>
-      <c r="E9" t="s" s="20">
-        <v>21</v>
-      </c>
-      <c r="F9" t="s" s="20">
+      <c r="E9" t="s" s="24">
         <v>22</v>
       </c>
-      <c r="G9" t="s" s="22">
+      <c r="F9" t="s" s="24">
         <v>23</v>
       </c>
-      <c r="H9" t="s" s="23">
+      <c r="G9" t="s" s="26">
         <v>24</v>
       </c>
-      <c r="I9" t="s" s="23">
+      <c r="H9" t="s" s="27">
         <v>25</v>
       </c>
-      <c r="J9" t="s" s="23">
+      <c r="I9" t="s" s="27">
         <v>26</v>
       </c>
-      <c r="K9" t="s" s="23">
+      <c r="J9" t="s" s="27">
         <v>27</v>
       </c>
-      <c r="L9" s="24">
+      <c r="K9" t="s" s="27">
+        <v>28</v>
+      </c>
+      <c r="L9" s="28">
         <v>1</v>
       </c>
-      <c r="M9" s="25">
+      <c r="M9" s="29">
         <v>500</v>
       </c>
-      <c r="N9" s="26">
+      <c r="N9" s="30">
         <v>500</v>
       </c>
-      <c r="O9" s="27"/>
-      <c r="P9" s="27"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+      <c r="Q9" t="s" s="31">
+        <v>29</v>
+      </c>
     </row>
     <row r="10" ht="22" customHeight="1">
-      <c r="A10" s="28"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="31"/>
-      <c r="O10" s="30"/>
-      <c r="P10" s="30"/>
+      <c r="A10" s="32">
+        <v>3535</v>
+      </c>
+      <c r="B10" s="33">
+        <v>6436436</v>
+      </c>
+      <c r="C10" t="s" s="34">
+        <v>21</v>
+      </c>
+      <c r="D10" s="35">
+        <v>44246</v>
+      </c>
+      <c r="E10" t="s" s="34">
+        <v>22</v>
+      </c>
+      <c r="F10" t="s" s="34">
+        <v>23</v>
+      </c>
+      <c r="G10" t="s" s="36">
+        <v>24</v>
+      </c>
+      <c r="H10" t="s" s="37">
+        <v>25</v>
+      </c>
+      <c r="I10" t="s" s="37">
+        <v>26</v>
+      </c>
+      <c r="J10" t="s" s="37">
+        <v>27</v>
+      </c>
+      <c r="K10" t="s" s="37">
+        <v>28</v>
+      </c>
+      <c r="L10" s="38">
+        <v>1</v>
+      </c>
+      <c r="M10" s="39">
+        <v>500</v>
+      </c>
+      <c r="N10" s="40">
+        <v>500</v>
+      </c>
+      <c r="O10" s="38"/>
+      <c r="P10" s="38"/>
+      <c r="Q10" t="s" s="41">
+        <v>30</v>
+      </c>
     </row>
     <row r="11" ht="22" customHeight="1">
-      <c r="A11" s="32"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="34"/>
-      <c r="M11" s="35"/>
-      <c r="N11" s="35"/>
-      <c r="O11" s="34"/>
-      <c r="P11" s="34"/>
+      <c r="A11" s="42"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="44"/>
+      <c r="M11" s="45"/>
+      <c r="N11" s="45"/>
+      <c r="O11" s="44"/>
+      <c r="P11" s="44"/>
+      <c r="Q11" s="44"/>
     </row>
     <row r="12" ht="22" customHeight="1">
-      <c r="A12" s="28"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="30"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="31"/>
-      <c r="O12" s="30"/>
-      <c r="P12" s="30"/>
+      <c r="A12" s="46"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="48"/>
+      <c r="M12" s="49"/>
+      <c r="N12" s="49"/>
+      <c r="O12" s="48"/>
+      <c r="P12" s="48"/>
+      <c r="Q12" s="48"/>
     </row>
     <row r="13" ht="22" customHeight="1">
-      <c r="A13" s="32"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="33"/>
-      <c r="L13" s="34"/>
-      <c r="M13" s="35"/>
-      <c r="N13" s="35"/>
-      <c r="O13" s="34"/>
-      <c r="P13" s="34"/>
+      <c r="A13" s="42"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="44"/>
+      <c r="M13" s="45"/>
+      <c r="N13" s="45"/>
+      <c r="O13" s="44"/>
+      <c r="P13" s="44"/>
+      <c r="Q13" s="44"/>
     </row>
     <row r="14" ht="22" customHeight="1">
-      <c r="A14" s="28"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="31"/>
-      <c r="N14" s="31"/>
-      <c r="O14" s="30"/>
-      <c r="P14" s="30"/>
+      <c r="A14" s="46"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="47"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="48"/>
+      <c r="M14" s="49"/>
+      <c r="N14" s="49"/>
+      <c r="O14" s="48"/>
+      <c r="P14" s="48"/>
+      <c r="Q14" s="48"/>
     </row>
     <row r="15" ht="22" customHeight="1">
-      <c r="A15" s="32"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
-      <c r="K15" s="33"/>
-      <c r="L15" s="34"/>
-      <c r="M15" s="35"/>
-      <c r="N15" s="35"/>
-      <c r="O15" s="34"/>
-      <c r="P15" s="34"/>
+      <c r="A15" s="42"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="44"/>
+      <c r="M15" s="45"/>
+      <c r="N15" s="45"/>
+      <c r="O15" s="44"/>
+      <c r="P15" s="44"/>
+      <c r="Q15" s="44"/>
     </row>
     <row r="16" ht="22" customHeight="1">
-      <c r="A16" s="28"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="30"/>
-      <c r="M16" s="31"/>
-      <c r="N16" s="31"/>
-      <c r="O16" s="30"/>
-      <c r="P16" s="30"/>
+      <c r="A16" s="46"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="48"/>
+      <c r="M16" s="49"/>
+      <c r="N16" s="49"/>
+      <c r="O16" s="48"/>
+      <c r="P16" s="48"/>
+      <c r="Q16" s="48"/>
     </row>
     <row r="17" ht="22" customHeight="1">
-      <c r="A17" s="32"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
-      <c r="K17" s="33"/>
-      <c r="L17" s="34"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="35"/>
-      <c r="O17" s="34"/>
-      <c r="P17" s="34"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="43"/>
+      <c r="L17" s="44"/>
+      <c r="M17" s="45"/>
+      <c r="N17" s="45"/>
+      <c r="O17" s="44"/>
+      <c r="P17" s="44"/>
+      <c r="Q17" s="44"/>
     </row>
     <row r="18" ht="22" customHeight="1">
-      <c r="A18" s="28"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="29"/>
-      <c r="L18" s="30"/>
-      <c r="M18" s="31"/>
-      <c r="N18" s="31"/>
-      <c r="O18" s="30"/>
-      <c r="P18" s="30"/>
+      <c r="A18" s="46"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
+      <c r="K18" s="47"/>
+      <c r="L18" s="48"/>
+      <c r="M18" s="49"/>
+      <c r="N18" s="49"/>
+      <c r="O18" s="48"/>
+      <c r="P18" s="48"/>
+      <c r="Q18" s="48"/>
     </row>
     <row r="19" ht="22" customHeight="1">
-      <c r="A19" s="32"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="33"/>
-      <c r="L19" s="34"/>
-      <c r="M19" s="35"/>
-      <c r="N19" s="35"/>
-      <c r="O19" s="34"/>
-      <c r="P19" s="34"/>
+      <c r="A19" s="42"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="44"/>
+      <c r="M19" s="45"/>
+      <c r="N19" s="45"/>
+      <c r="O19" s="44"/>
+      <c r="P19" s="44"/>
+      <c r="Q19" s="44"/>
     </row>
     <row r="20" ht="22" customHeight="1">
-      <c r="A20" s="28"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="30"/>
-      <c r="M20" s="31"/>
-      <c r="N20" s="31"/>
-      <c r="O20" s="30"/>
-      <c r="P20" s="30"/>
+      <c r="A20" s="46"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="47"/>
+      <c r="J20" s="47"/>
+      <c r="K20" s="47"/>
+      <c r="L20" s="48"/>
+      <c r="M20" s="49"/>
+      <c r="N20" s="49"/>
+      <c r="O20" s="48"/>
+      <c r="P20" s="48"/>
+      <c r="Q20" s="48"/>
     </row>
     <row r="21" ht="22" customHeight="1">
-      <c r="A21" s="32"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="34"/>
-      <c r="M21" s="35"/>
-      <c r="N21" s="35"/>
-      <c r="O21" s="34"/>
-      <c r="P21" s="34"/>
+      <c r="A21" s="42"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="43"/>
+      <c r="K21" s="43"/>
+      <c r="L21" s="44"/>
+      <c r="M21" s="45"/>
+      <c r="N21" s="45"/>
+      <c r="O21" s="44"/>
+      <c r="P21" s="44"/>
+      <c r="Q21" s="44"/>
     </row>
     <row r="22" ht="22" customHeight="1">
-      <c r="A22" s="28"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="29"/>
-      <c r="L22" s="30"/>
-      <c r="M22" s="31"/>
-      <c r="N22" s="31"/>
-      <c r="O22" s="30"/>
-      <c r="P22" s="30"/>
+      <c r="A22" s="46"/>
+      <c r="B22" s="47"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="47"/>
+      <c r="J22" s="47"/>
+      <c r="K22" s="47"/>
+      <c r="L22" s="48"/>
+      <c r="M22" s="49"/>
+      <c r="N22" s="49"/>
+      <c r="O22" s="48"/>
+      <c r="P22" s="48"/>
+      <c r="Q22" s="48"/>
     </row>
     <row r="23" ht="23" customHeight="1">
-      <c r="A23" s="36"/>
-      <c r="B23" s="37"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="37"/>
-      <c r="J23" s="37"/>
-      <c r="K23" s="37"/>
-      <c r="L23" s="38"/>
-      <c r="M23" s="39"/>
-      <c r="N23" s="39"/>
-      <c r="O23" s="38"/>
-      <c r="P23" s="38"/>
+      <c r="A23" s="50"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="51"/>
+      <c r="L23" s="52"/>
+      <c r="M23" s="53"/>
+      <c r="N23" s="53"/>
+      <c r="O23" s="52"/>
+      <c r="P23" s="52"/>
+      <c r="Q23" s="52"/>
     </row>
     <row r="24" ht="23" customHeight="1">
-      <c r="A24" s="40"/>
-      <c r="B24" s="41"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="41"/>
-      <c r="G24" s="41"/>
-      <c r="H24" s="41"/>
-      <c r="I24" s="41"/>
-      <c r="J24" s="41"/>
-      <c r="K24" s="41"/>
-      <c r="L24" t="s" s="42">
-        <v>28</v>
-      </c>
-      <c r="M24" s="43">
+      <c r="A24" s="54"/>
+      <c r="B24" s="55"/>
+      <c r="C24" s="55"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="55"/>
+      <c r="G24" s="55"/>
+      <c r="H24" s="55"/>
+      <c r="I24" s="55"/>
+      <c r="J24" s="55"/>
+      <c r="K24" s="55"/>
+      <c r="L24" t="s" s="56">
+        <v>31</v>
+      </c>
+      <c r="M24" s="57">
         <v>10000</v>
       </c>
-      <c r="N24" s="43">
+      <c r="N24" s="57">
         <v>10000</v>
       </c>
-      <c r="O24" s="44"/>
-      <c r="P24" s="44"/>
+      <c r="O24" s="58"/>
+      <c r="P24" s="58"/>
+      <c r="Q24" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A7:P7"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A6:P6"/>
+    <mergeCell ref="A5:P5"/>
+    <mergeCell ref="A4:P4"/>
     <mergeCell ref="A3:P3"/>
     <mergeCell ref="A2:P2"/>
-    <mergeCell ref="A4:P4"/>
-    <mergeCell ref="A5:P5"/>
-    <mergeCell ref="A6:P6"/>
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A7:P7"/>
   </mergeCells>
-  <conditionalFormatting sqref="A9:P24">
+  <conditionalFormatting sqref="A9:Q9 A11:Q24">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal" stopIfTrue="1">
+      <formula>"F"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10:Q10">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal" stopIfTrue="1">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>